<commit_message>
On droplet changes to queries and data
</commit_message>
<xml_diff>
--- a/data/abuse/cell_list.xlsx
+++ b/data/abuse/cell_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeange\PycharmProjects\batteryarchive-agent\data\abuse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeange\Documents\BA\ORNL-SNL-Abuse-Data\SNL_Indentation_Data_220829_import\abuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E665F0-16B6-4E40-BFE6-42645999A090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A0BC82-7A9B-4CDA-BE97-0C52F721DBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07EF3D65-9BA3-43DB-B014-0F8C59FBB292}"/>
+    <workbookView xWindow="9615" yWindow="-17610" windowWidth="29235" windowHeight="11385" xr2:uid="{7F981527-D12A-432F-9635-60B17A59881B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,100 +33,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
-  <si>
-    <t>NMC</t>
-  </si>
-  <si>
-    <t>graphite</t>
-  </si>
-  <si>
-    <t>commercial</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">Pouch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphite </t>
+  </si>
+  <si>
+    <t>SNL_LFP_Graphite_10Ah_100SOC_a</t>
+  </si>
+  <si>
+    <t>SNL_LFP_Graphite_10Ah_100SOC_b</t>
+  </si>
+  <si>
+    <t>LFP</t>
+  </si>
+  <si>
+    <t>9 × 93 × 163</t>
+  </si>
+  <si>
+    <t>cell_id</t>
   </si>
   <si>
     <t>file_id</t>
   </si>
   <si>
-    <t>cell_id</t>
-  </si>
-  <si>
     <t>cathode</t>
   </si>
   <si>
     <t>anode</t>
   </si>
   <si>
-    <t>temperature</t>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>form_factor</t>
+  </si>
+  <si>
+    <t>dimensions</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>indentor</t>
+  </si>
+  <si>
+    <t>nail_speed</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>soc</t>
+  </si>
+  <si>
+    <t>v_init</t>
   </si>
   <si>
     <t>source</t>
   </si>
   <si>
-    <t>ah</t>
-  </si>
-  <si>
-    <t>form_factor</t>
-  </si>
-  <si>
-    <t>tester</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
     <t>abuse</t>
   </si>
   <si>
-    <t>file_type</t>
-  </si>
-  <si>
-    <t>thickness</t>
-  </si>
-  <si>
-    <t>pouch</t>
-  </si>
-  <si>
-    <t>xlsx</t>
-  </si>
-  <si>
-    <t>snl</t>
-  </si>
-  <si>
-    <t>ornl</t>
-  </si>
-  <si>
-    <t>v_init</t>
-  </si>
-  <si>
-    <t>indentor</t>
-  </si>
-  <si>
-    <t>nail_speed</t>
-  </si>
-  <si>
-    <t>mapping</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>ORNL_abuse</t>
-  </si>
-  <si>
-    <t>SNL_abuse</t>
-  </si>
-  <si>
-    <t>ORNL_Abuse</t>
-  </si>
-  <si>
-    <t>SNL_Abuse</t>
+    <t xml:space="preserve">SNL-Hydraulic </t>
+  </si>
+  <si>
+    <t>Battery Space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +121,22 @@
     </font>
     <font>
       <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,36 +150,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -191,12 +164,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,181 +489,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4900B09B-8105-4727-A8D5-7A7308C12DCF}">
-  <dimension ref="A1:X3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CC2AF5-6EA1-427A-83DC-157FCE0DBCEE}">
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="38" customWidth="1"/>
+    <col min="3" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3">
-        <v>26</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>16</v>
+      <c r="E2" s="3">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="H2" s="3">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="I2" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2" s="3">
-        <v>4.12</v>
-      </c>
-      <c r="K2" s="3">
-        <v>6</v>
+        <v>0.05</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="L2" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>24</v>
+        <v>100</v>
+      </c>
+      <c r="M2" s="3">
+        <v>3.3980000000000001</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>26</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
+      <c r="E3" s="3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="I3" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J3" s="3">
-        <v>4.18</v>
-      </c>
-      <c r="K3" s="3">
-        <v>6</v>
+        <v>0.05</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="L3" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M3" s="3">
+        <v>3.403</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>